<commit_message>
Appending similar quantities (column names) to the appropriate subsection in Tabular_Parser
In the excel sheet/excel file, when exactly similar column names exists, then, in the row mode only, for the quantity that refers to those columns (via assigning proper tabular annotation), each column (section) is appended to the appropriate (repeating) subsection.

Changelog: Added
</commit_message>
<xml_diff>
--- a/tests/data/parsers/tabular/Test.xlsx
+++ b/tests/data/parsers/tabular/Test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26216"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0796B8ED-8B16-4403-9C15-51DE9B2E6122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D112209-2919-4A61-89D9-5D67337846F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_1" sheetId="1" r:id="rId1"/>
     <sheet name="sheet_2" sheetId="6" r:id="rId2"/>
+    <sheet name="sheet_3" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>########## start Header ##########</t>
   </si>
@@ -53,6 +54,36 @@
   </si>
   <si>
     <t>column_3</t>
+  </si>
+  <si>
+    <t>quantity_1</t>
+  </si>
+  <si>
+    <t>quantity_2</t>
+  </si>
+  <si>
+    <t>q1_d0_r0</t>
+  </si>
+  <si>
+    <t>q1_d1_r0</t>
+  </si>
+  <si>
+    <t>q2_d0_r0</t>
+  </si>
+  <si>
+    <t>q2_d1_r0</t>
+  </si>
+  <si>
+    <t>q1_d0_r1</t>
+  </si>
+  <si>
+    <t>q1_d1_r1</t>
+  </si>
+  <si>
+    <t>q2_d0_r1</t>
+  </si>
+  <si>
+    <t>q2_d1_r1</t>
   </si>
 </sst>
 </file>
@@ -60,9 +91,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -114,16 +145,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -513,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection sqref="A1:A7"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="14.25"/>
@@ -868,4 +899,64 @@
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E552DF16-3577-4598-B888-A82F40109090}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added `root` mode to the tabular parser to enable more generalized usage of mixed column/row modes
When top section is inheriting from TableData, all the subsections should adhere to the same mode of the top section. Now the top section can be of type `root`, allowing the subsections to be of type column or row (independent of one another).

Changelog: Added
</commit_message>
<xml_diff>
--- a/tests/data/parsers/tabular/Test.xlsx
+++ b/tests/data/parsers/tabular/Test.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26216"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26301"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D112209-2919-4A61-89D9-5D67337846F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A1BCC8C-AD4D-4BB9-BA7B-75883EBA4C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_1" sheetId="1" r:id="rId1"/>
     <sheet name="sheet_2" sheetId="6" r:id="rId2"/>
     <sheet name="sheet_3" sheetId="7" r:id="rId3"/>
+    <sheet name="sheet_4" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>########## start Header ##########</t>
   </si>
@@ -84,6 +85,63 @@
   </si>
   <si>
     <t>q2_d1_r1</t>
+  </si>
+  <si>
+    <t># comments</t>
+  </si>
+  <si>
+    <t>Header 1</t>
+  </si>
+  <si>
+    <t>Header 2</t>
+  </si>
+  <si>
+    <t>Header 3</t>
+  </si>
+  <si>
+    <t>Header 4</t>
+  </si>
+  <si>
+    <t>Header 5</t>
+  </si>
+  <si>
+    <t>Header 6</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>my_str1</t>
+  </si>
+  <si>
+    <t>test11</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>my_str2</t>
+  </si>
+  <si>
+    <t>test12</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>my_str3</t>
+  </si>
+  <si>
+    <t>test13</t>
   </si>
 </sst>
 </file>
@@ -95,7 +153,7 @@
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -110,6 +168,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
@@ -134,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -160,6 +224,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -905,7 +970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E552DF16-3577-4598-B888-A82F40109090}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -959,4 +1024,165 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14275015-9F09-4E8F-92B9-A94522E02BE8}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="9">
+        <v>11</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="9">
+        <v>12</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="9">
+        <v>13</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added entry mode to follow the same workflow as the column/row modes in tabular parser
Entry mode was originally working as a parser, but now one can use it the same way as the column- or row-mode is being utilized in tabular parser.

Changelog: Added
</commit_message>
<xml_diff>
--- a/tests/data/parsers/tabular/Test.xlsx
+++ b/tests/data/parsers/tabular/Test.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26301"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26312"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A1BCC8C-AD4D-4BB9-BA7B-75883EBA4C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9841FDF2-9349-4CEF-A474-8DBBF44FEBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet_1" sheetId="1" r:id="rId1"/>

</xml_diff>